<commit_message>
changes to experiment (including vlc update) + data
</commit_message>
<xml_diff>
--- a/behavioral_August2019/story_xlsx_files_RECORDED/11.xlsx
+++ b/behavioral_August2019/story_xlsx_files_RECORDED/11.xlsx
@@ -44,45 +44,73 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">A bell chimed as the door swung open, and Sadie entered to find Thomas, who was </t>
+      <t>A bell chimed as the door swung open, and Sadie entered to find Thomas, who was dreading the approaching breakup conversation he was about to start, ruminating at the bar.</t>
     </r>
+  </si>
+  <si>
+    <t>Thomas had been thinking about breaking up with her for 2 months now.</t>
+  </si>
+  <si>
+    <t>The restaurant he had chosen to meet at was reminiscent of a diner from the 70’s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There was black and white checkerboard tiling on the floor, a long bar in the front, and booths and stools with red, leather upholstery. </t>
+  </si>
+  <si>
+    <t>Thomas stood up and gave Sadie a side hug, asking quickly, “How was your day?”</t>
+  </si>
+  <si>
+    <t>She clung onto him, “It was okay- I missed you today.”</t>
+  </si>
+  <si>
+    <t>He looked away and addressed the hostess coming towards them, “Can we have a booth in the back?”</t>
+  </si>
+  <si>
+    <t>She shrugged and after loudly popping her bubblegum replied, “Sure, honey.”</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="16"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>dreading the approaching breakup conversation he was about to start,</t>
+      <t xml:space="preserve">The hostess seated them at a booth in the back corner of the diner.  </t>
     </r>
+  </si>
+  <si>
+    <t>Sadie slipped into the cushioned seat and grabbed Thomas’ hand.</t>
+  </si>
+  <si>
+    <t>“Tell me about your day!” she sang.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas looked away and took a deep breath. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sadie asked, “What’s wrong?” </t>
+  </si>
+  <si>
+    <t>Thomas picked at his fingernails.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="16"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve"> ruminating at the bar.</t>
+      <t>After a few moments, Thomas let out a deep breath and said, “Sadie, I’ve been thinking, and I need a break from this relationship because I need to figure out my career path on my own.”</t>
     </r>
   </si>
   <si>
-    <t>Thomas had been thinking about breaking up with her for 2 months now.</t>
-  </si>
-  <si>
-    <t>The restaurant he had chosen to meet at was reminiscent of a diner from the 70’s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There were black and white checkerboard tiling on the floor, a long bar in the front, and booths and stools with red, leather upholstery. </t>
-  </si>
-  <si>
-    <t>Thomas stood up and gave Sadie a side hug, asking quickly, “How was your day?”</t>
-  </si>
-  <si>
-    <t>She clung onto him, “It was okay- I missed you today.”</t>
-  </si>
-  <si>
-    <t>He looked away and addressed the hostess coming towards them, “Can we have a booth in the back?”</t>
-  </si>
-  <si>
-    <t>She shrugged and after loudly popping her bubblegum replied, “Sure, honey.”</t>
+    <t>Sadie sat back in her seat.</t>
+  </si>
+  <si>
+    <t>Thomas continued, “Things have been really picking up at work, and I’m not sure that this is the job I want to do anymore.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plus, it’s been really overwhelming between working and figuring out if I should change careers, and I really feel like I need more time to figure it out.” </t>
   </si>
   <si>
     <r>
@@ -91,91 +119,7 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>The hostess</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> seated them at a booth in the back corner of the diner.  </t>
-    </r>
-  </si>
-  <si>
-    <t>Sadie slipped into the cushioned seat and grabbed Thomas’ hand.</t>
-  </si>
-  <si>
-    <t>“Tell me about your day!” she sang.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thomas looked away and took a deep breath. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sadie asked, “What’s wrong?” </t>
-  </si>
-  <si>
-    <t>Thomas picked at his fingernails.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">After a few moments, Thomas let out a deep breath and said, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>“Sadie, I’ve been thinking, and I need a break from this relationship because I need to figure out my career path on my own.”</t>
-    </r>
-  </si>
-  <si>
-    <t>Sadie sat back in her seat.</t>
-  </si>
-  <si>
-    <t>Thomas continued, “Things have been really picking up at work, and I’m not sure that this is the job I want to do anymore.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plus, it’s been really overwhelming between working and figuring out if I should change careers, and I really feel like I need more time to figure it out.” </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">he waiter appeared and cheerily asked, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>“</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Have you decided what you would like?”</t>
+      <t>The waiter appeared and cheerily asked, “Have you decided what you would like?”</t>
     </r>
   </si>
   <si>
@@ -228,34 +172,45 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">Sadie- not so </t>
+      <t xml:space="preserve">Sadie- not so quietly- burst into tears. </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">People sitting at the bar looked over and quickly averted their gaze when they figured what was happening. </t>
+  </si>
+  <si>
+    <t>She whispered, “Is this really what you want?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I don’t understand- things were fine, I thought. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think we should stay together because we can change how much we hang out. </t>
+  </si>
+  <si>
+    <t>We don’t have to hang out all the time, or as much as we do now.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas chewed on his bottom lip and picked at his now bleeding hangnail. </t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="16"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">quietly- burst into tears. </t>
+      <t>The waiter appeared with the burger and reuben and set them in front of them.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">People sitting at the bar looked over and quickly averted their gaze when they figured what was happening. </t>
-  </si>
-  <si>
-    <t>She whispered, “Is this really what you want?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I don’t understand- things were fine, I thought. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I think we should stay together because we can change how much we hang out. </t>
-  </si>
-  <si>
-    <t>We don’t have to hang out all the time, or as much as we do now.”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thomas chewed on his bottom lip and picked at his now bleeding hangnail. </t>
+    <t>“Is there anything else I can get for you two?</t>
+  </si>
+  <si>
+    <t>Will you be getting dessert tonight?” he asked.</t>
+  </si>
+  <si>
+    <t>“Oh no, we’re good, thanks,” said Thomas blankly.</t>
   </si>
   <si>
     <r>
@@ -264,42 +219,7 @@
         <color indexed="8"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>he waiter appeared with the burger and reuben and set them in front of them.</t>
-    </r>
-  </si>
-  <si>
-    <t>“Is there anything else I can get for you two?</t>
-  </si>
-  <si>
-    <t>Will you be getting dessert tonight?” he asked.</t>
-  </si>
-  <si>
-    <t>“Oh no, we’re good, thanks,” Thomas said blankly.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>With the waiter gone, Sadie suddenly</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> stood up, grabbed half of the reuben, and shook it at him as she growled, “Don’t follow me, and don’t talk to me anymore!</t>
+      <t>With the waiter gone, Sadie suddenly stood up, grabbed half of the reuben, and shook it at him as she growled, “Don’t follow me, and don’t talk to me anymore!</t>
     </r>
   </si>
   <si>
@@ -325,7 +245,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -334,7 +254,12 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue Medium"/>
     </font>
     <font>
       <b val="1"/>
@@ -348,7 +273,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,6 +289,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -487,44 +418,38 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -548,6 +473,7 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -564,10 +490,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -596,14 +522,14 @@
     </a:clrScheme>
     <a:fontScheme name="Blank">
       <a:majorFont>
-        <a:latin typeface="Helvetica Neue"/>
-        <a:ea typeface="Helvetica Neue"/>
-        <a:cs typeface="Helvetica Neue"/>
+        <a:latin typeface="Helvetica"/>
+        <a:ea typeface="Helvetica"/>
+        <a:cs typeface="Helvetica"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Helvetica Neue"/>
-        <a:ea typeface="Helvetica Neue"/>
-        <a:cs typeface="Helvetica Neue"/>
+        <a:latin typeface="Helvetica"/>
+        <a:ea typeface="Helvetica"/>
+        <a:cs typeface="Helvetica"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Blank">
@@ -744,11 +670,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -757,33 +686,33 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Helvetica Neue"/>
+            <a:ea typeface="Helvetica Neue"/>
+            <a:cs typeface="Helvetica Neue"/>
             <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
@@ -1034,10 +963,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1328,7 +1257,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1352,9 +1281,9 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
+            <a:latin typeface="Helvetica Neue"/>
+            <a:ea typeface="Helvetica Neue"/>
+            <a:cs typeface="Helvetica Neue"/>
             <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
@@ -1611,13 +1540,11 @@
   </sheetPr>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="165.242" style="1" customWidth="1"/>
+    <col min="1" max="1" width="165.352" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
@@ -1666,716 +1593,716 @@
       <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="6">
         <v>11</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="8">
+      <c r="A3" t="s" s="7">
         <v>9</v>
       </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="10">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="10">
-        <v>1</v>
-      </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="8">
+      <c r="A4" t="s" s="7">
         <v>10</v>
       </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10">
-        <v>1</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="10">
-        <v>1</v>
-      </c>
-      <c r="I4" s="11"/>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="8">
+      <c r="A5" t="s" s="7">
         <v>11</v>
       </c>
-      <c r="B5" s="9">
-        <v>1</v>
-      </c>
-      <c r="C5" s="10">
-        <v>1</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" ht="25.8" customHeight="1">
-      <c r="A6" t="s" s="12">
+      <c r="A6" t="s" s="10">
         <v>12</v>
       </c>
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="10">
-        <v>1</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" ht="25.8" customHeight="1">
-      <c r="A7" t="s" s="12">
+      <c r="A7" t="s" s="10">
         <v>13</v>
       </c>
-      <c r="B7" s="9">
-        <v>1</v>
-      </c>
-      <c r="C7" s="10">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" ht="25.8" customHeight="1">
-      <c r="A8" t="s" s="12">
+      <c r="A8" t="s" s="10">
         <v>14</v>
       </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
-      <c r="C8" s="10">
-        <v>1</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" ht="25.8" customHeight="1">
-      <c r="A9" t="s" s="12">
+      <c r="A9" t="s" s="10">
         <v>15</v>
       </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="10">
-        <v>1</v>
-      </c>
-      <c r="D9" s="10">
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
         <v>9</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" ht="25.8" customHeight="1">
-      <c r="A10" t="s" s="8">
+      <c r="A10" t="s" s="7">
         <v>16</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>2</v>
       </c>
-      <c r="C10" s="10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" ht="25.8" customHeight="1">
-      <c r="A11" t="s" s="12">
+      <c r="A11" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>2</v>
       </c>
-      <c r="C11" s="10">
-        <v>1</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" ht="25.8" customHeight="1">
-      <c r="A12" t="s" s="12">
+      <c r="A12" t="s" s="10">
         <v>18</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>2</v>
       </c>
-      <c r="C12" s="10">
-        <v>1</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" ht="25.8" customHeight="1">
-      <c r="A13" t="s" s="12">
+      <c r="A13" t="s" s="10">
         <v>19</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>2</v>
       </c>
-      <c r="C13" s="10">
-        <v>1</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" ht="25.8" customHeight="1">
-      <c r="A14" t="s" s="12">
+      <c r="A14" t="s" s="10">
         <v>20</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>2</v>
       </c>
-      <c r="C14" s="10">
-        <v>1</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" ht="25.8" customHeight="1">
-      <c r="A15" t="s" s="12">
+      <c r="A15" t="s" s="10">
         <v>21</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>2</v>
       </c>
-      <c r="C15" s="10">
-        <v>1</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10">
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9">
         <v>22</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" ht="43.8" customHeight="1">
-      <c r="A16" t="s" s="12">
+      <c r="A16" t="s" s="10">
         <v>22</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="8">
         <v>2</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <v>2</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" ht="25.8" customHeight="1">
-      <c r="A17" t="s" s="12">
+      <c r="A17" t="s" s="10">
         <v>23</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="8">
         <v>2</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>2</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" ht="25.8" customHeight="1">
-      <c r="A18" t="s" s="12">
+      <c r="A18" t="s" s="10">
         <v>24</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="8">
         <v>2</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <v>2</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
     </row>
     <row r="19" ht="43.8" customHeight="1">
-      <c r="A19" t="s" s="12">
+      <c r="A19" t="s" s="10">
         <v>25</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="8">
         <v>2</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <v>2</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <v>17</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" ht="25.8" customHeight="1">
-      <c r="A20" t="s" s="12">
+      <c r="A20" t="s" s="10">
         <v>26</v>
       </c>
-      <c r="B20" s="9">
-        <v>3</v>
-      </c>
-      <c r="C20" s="10">
+      <c r="B20" s="8">
+        <v>3</v>
+      </c>
+      <c r="C20" s="9">
         <v>2</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" ht="25.8" customHeight="1">
-      <c r="A21" t="s" s="12">
+      <c r="A21" t="s" s="10">
         <v>27</v>
       </c>
-      <c r="B21" s="9">
-        <v>3</v>
-      </c>
-      <c r="C21" s="10">
+      <c r="B21" s="8">
+        <v>3</v>
+      </c>
+      <c r="C21" s="9">
         <v>2</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
     </row>
     <row r="22" ht="43.8" customHeight="1">
-      <c r="A22" t="s" s="12">
+      <c r="A22" t="s" s="10">
         <v>28</v>
       </c>
-      <c r="B22" s="9">
-        <v>3</v>
-      </c>
-      <c r="C22" s="10">
+      <c r="B22" s="8">
+        <v>3</v>
+      </c>
+      <c r="C22" s="9">
         <v>2</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
     </row>
     <row r="23" ht="25.8" customHeight="1">
-      <c r="A23" t="s" s="12">
+      <c r="A23" t="s" s="10">
         <v>29</v>
       </c>
-      <c r="B23" s="9">
-        <v>3</v>
-      </c>
-      <c r="C23" s="10">
+      <c r="B23" s="8">
+        <v>3</v>
+      </c>
+      <c r="C23" s="9">
         <v>2</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" ht="25.8" customHeight="1">
-      <c r="A24" t="s" s="12">
+      <c r="A24" t="s" s="10">
         <v>30</v>
       </c>
-      <c r="B24" s="9">
-        <v>3</v>
-      </c>
-      <c r="C24" s="10">
+      <c r="B24" s="8">
+        <v>3</v>
+      </c>
+      <c r="C24" s="9">
         <v>2</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
     </row>
     <row r="25" ht="25.8" customHeight="1">
-      <c r="A25" t="s" s="12">
+      <c r="A25" t="s" s="10">
         <v>31</v>
       </c>
-      <c r="B25" s="9">
-        <v>3</v>
-      </c>
-      <c r="C25" s="10">
+      <c r="B25" s="8">
+        <v>3</v>
+      </c>
+      <c r="C25" s="9">
         <v>2</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
     </row>
     <row r="26" ht="25.8" customHeight="1">
-      <c r="A26" t="s" s="12">
+      <c r="A26" t="s" s="10">
         <v>32</v>
       </c>
-      <c r="B26" s="9">
-        <v>3</v>
-      </c>
-      <c r="C26" s="10">
-        <v>3</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
+      <c r="B26" s="8">
+        <v>3</v>
+      </c>
+      <c r="C26" s="9">
+        <v>3</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
     </row>
     <row r="27" ht="25.8" customHeight="1">
-      <c r="A27" t="s" s="12">
+      <c r="A27" t="s" s="10">
         <v>33</v>
       </c>
-      <c r="B27" s="9">
-        <v>3</v>
-      </c>
-      <c r="C27" s="10">
-        <v>3</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
+      <c r="B27" s="8">
+        <v>3</v>
+      </c>
+      <c r="C27" s="9">
+        <v>3</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
     </row>
     <row r="28" ht="25.8" customHeight="1">
-      <c r="A28" t="s" s="12">
+      <c r="A28" t="s" s="10">
         <v>34</v>
       </c>
-      <c r="B28" s="9">
-        <v>3</v>
-      </c>
-      <c r="C28" s="10">
-        <v>3</v>
-      </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
+      <c r="B28" s="8">
+        <v>3</v>
+      </c>
+      <c r="C28" s="9">
+        <v>3</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
     </row>
     <row r="29" ht="25.8" customHeight="1">
-      <c r="A29" t="s" s="12">
+      <c r="A29" t="s" s="10">
         <v>35</v>
       </c>
-      <c r="B29" s="9">
-        <v>3</v>
-      </c>
-      <c r="C29" s="10">
-        <v>3</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
+      <c r="B29" s="8">
+        <v>3</v>
+      </c>
+      <c r="C29" s="9">
+        <v>3</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
     </row>
     <row r="30" ht="25.8" customHeight="1">
-      <c r="A30" t="s" s="12">
+      <c r="A30" t="s" s="10">
         <v>36</v>
       </c>
-      <c r="B30" s="9">
-        <v>3</v>
-      </c>
-      <c r="C30" s="10">
-        <v>3</v>
-      </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
+      <c r="B30" s="8">
+        <v>3</v>
+      </c>
+      <c r="C30" s="9">
+        <v>3</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
     </row>
     <row r="31" ht="25.8" customHeight="1">
-      <c r="A31" t="s" s="12">
+      <c r="A31" t="s" s="10">
         <v>37</v>
       </c>
-      <c r="B31" s="9">
-        <v>3</v>
-      </c>
-      <c r="C31" s="10">
-        <v>3</v>
-      </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
+      <c r="B31" s="8">
+        <v>3</v>
+      </c>
+      <c r="C31" s="9">
+        <v>3</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32" ht="25.8" customHeight="1">
-      <c r="A32" t="s" s="12">
+      <c r="A32" t="s" s="10">
         <v>38</v>
       </c>
-      <c r="B32" s="9">
-        <v>3</v>
-      </c>
-      <c r="C32" s="10">
-        <v>3</v>
-      </c>
-      <c r="D32" s="10">
+      <c r="B32" s="8">
+        <v>3</v>
+      </c>
+      <c r="C32" s="9">
+        <v>3</v>
+      </c>
+      <c r="D32" s="9">
         <v>20</v>
       </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
     </row>
     <row r="33" ht="25.8" customHeight="1">
-      <c r="A33" t="s" s="12">
+      <c r="A33" t="s" s="10">
         <v>39</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="8">
         <v>4</v>
       </c>
-      <c r="C33" s="10">
-        <v>3</v>
-      </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
+      <c r="C33" s="9">
+        <v>3</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
     </row>
     <row r="34" ht="25.8" customHeight="1">
-      <c r="A34" t="s" s="12">
+      <c r="A34" t="s" s="10">
         <v>40</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="8">
         <v>4</v>
       </c>
-      <c r="C34" s="10">
-        <v>3</v>
-      </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
+      <c r="C34" s="9">
+        <v>3</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
     </row>
     <row r="35" ht="25.8" customHeight="1">
-      <c r="A35" t="s" s="12">
+      <c r="A35" t="s" s="10">
         <v>41</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="8">
         <v>4</v>
       </c>
-      <c r="C35" s="10">
-        <v>3</v>
-      </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
+      <c r="C35" s="9">
+        <v>3</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
     </row>
     <row r="36" ht="25.8" customHeight="1">
-      <c r="A36" t="s" s="12">
+      <c r="A36" t="s" s="10">
         <v>42</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="8">
         <v>4</v>
       </c>
-      <c r="C36" s="10">
-        <v>3</v>
-      </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
+      <c r="C36" s="9">
+        <v>3</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
     </row>
     <row r="37" ht="43.8" customHeight="1">
-      <c r="A37" t="s" s="12">
+      <c r="A37" t="s" s="10">
         <v>43</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="8">
         <v>4</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="9">
         <v>4</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
     </row>
     <row r="38" ht="25.8" customHeight="1">
-      <c r="A38" t="s" s="12">
+      <c r="A38" t="s" s="10">
         <v>44</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="8">
         <v>4</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="9">
         <v>4</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
     </row>
     <row r="39" ht="25.8" customHeight="1">
-      <c r="A39" t="s" s="12">
+      <c r="A39" t="s" s="10">
         <v>45</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="8">
         <v>4</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="9">
         <v>4</v>
       </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
     </row>
     <row r="40" ht="25.8" customHeight="1">
-      <c r="A40" t="s" s="12">
+      <c r="A40" t="s" s="10">
         <v>46</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="8">
         <v>4</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="9">
         <v>4</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
     </row>
     <row r="41" ht="25.8" customHeight="1">
-      <c r="A41" t="s" s="12">
+      <c r="A41" t="s" s="10">
         <v>47</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="8">
         <v>4</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="9">
         <v>4</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
     </row>
     <row r="42" ht="25.8" customHeight="1">
-      <c r="A42" t="s" s="12">
+      <c r="A42" t="s" s="10">
         <v>48</v>
       </c>
-      <c r="B42" s="9">
+      <c r="B42" s="8">
         <v>4</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="9">
         <v>4</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="9">
         <v>13</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="9">
         <v>5</v>
       </c>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
big changes, adding fMRI task
</commit_message>
<xml_diff>
--- a/behavioral_August2019/story_xlsx_files_RECORDED/11.xlsx
+++ b/behavioral_August2019/story_xlsx_files_RECORDED/11.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+  <si>
+    <t>sentence number</t>
+  </si>
   <si>
     <t>storyText</t>
   </si>
@@ -36,6 +39,9 @@
   </si>
   <si>
     <t>story</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <r>
@@ -299,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -319,6 +325,21 @@
       </top>
       <bottom style="thin">
         <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -360,7 +381,7 @@
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -399,10 +420,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
@@ -418,7 +439,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -434,22 +455,34 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -710,10 +743,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue"/>
-            <a:ea typeface="Helvetica Neue"/>
-            <a:cs typeface="Helvetica Neue"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1281,10 +1314,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue"/>
-            <a:ea typeface="Helvetica Neue"/>
-            <a:cs typeface="Helvetica Neue"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1538,14 +1571,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="165.352" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15" style="1" customWidth="1"/>
+    <col min="2" max="2" width="165.352" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
@@ -1553,7 +1586,8 @@
     <col min="7" max="7" width="16.3516" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.3516" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.3516" style="1" customWidth="1"/>
-    <col min="10" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.3516" style="1" customWidth="1"/>
+    <col min="11" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1572,731 +1606,897 @@
       <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" t="s" s="2">
+      <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
+      <c r="G1" s="3"/>
       <c r="H1" t="s" s="2">
         <v>6</v>
       </c>
       <c r="I1" t="s" s="2">
         <v>7</v>
       </c>
+      <c r="J1" t="s" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" ht="44" customHeight="1">
       <c r="A2" t="s" s="4">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="s" s="5">
+        <v>10</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6">
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7">
         <v>11</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="7">
+      <c r="A3" s="8">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="9">
+        <v>11</v>
+      </c>
+      <c r="C3" s="10">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11">
+        <v>1</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" s="12">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11">
+        <v>1</v>
+      </c>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" s="12">
+        <f>A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="13">
+        <v>13</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" ht="25.8" customHeight="1">
+      <c r="A6" s="12">
+        <f>A5+1</f>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s" s="14">
+        <v>14</v>
+      </c>
+      <c r="C6" s="10">
+        <v>1</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" ht="25.8" customHeight="1">
+      <c r="A7" s="12">
+        <f>A6+1</f>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s" s="14">
+        <v>15</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" ht="25.8" customHeight="1">
+      <c r="A8" s="12">
+        <f>A7+1</f>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="C8" s="10">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" ht="25.8" customHeight="1">
+      <c r="A9" s="12">
+        <f>A8+1</f>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s" s="14">
+        <v>17</v>
+      </c>
+      <c r="C9" s="10">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11">
         <v>9</v>
       </c>
-      <c r="B3" s="8">
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" ht="25.8" customHeight="1">
+      <c r="A10" s="12">
+        <f>A9+1</f>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s" s="13">
+        <v>18</v>
+      </c>
+      <c r="C10" s="10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="9">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" ht="25.8" customHeight="1">
+      <c r="A11" s="12">
+        <f>A10+1</f>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s" s="14">
+        <v>19</v>
+      </c>
+      <c r="C11" s="10">
+        <v>2</v>
+      </c>
+      <c r="D11" s="11">
         <v>1</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" ht="25.8" customHeight="1">
+      <c r="A12" s="12">
+        <f>A11+1</f>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="C12" s="10">
+        <v>2</v>
+      </c>
+      <c r="D12" s="11">
         <v>1</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="B4" s="8">
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" ht="25.8" customHeight="1">
+      <c r="A13" s="12">
+        <f>A12+1</f>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s" s="14">
+        <v>21</v>
+      </c>
+      <c r="C13" s="10">
+        <v>2</v>
+      </c>
+      <c r="D13" s="11">
         <v>1</v>
       </c>
-      <c r="C4" s="9">
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" ht="25.8" customHeight="1">
+      <c r="A14" s="12">
+        <f>A13+1</f>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s" s="14">
+        <v>22</v>
+      </c>
+      <c r="C14" s="10">
+        <v>2</v>
+      </c>
+      <c r="D14" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" ht="25.8" customHeight="1">
+      <c r="A15" s="12">
+        <f>A14+1</f>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s" s="14">
+        <v>23</v>
+      </c>
+      <c r="C15" s="10">
+        <v>2</v>
+      </c>
+      <c r="D15" s="11">
         <v>1</v>
       </c>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="7">
-        <v>11</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" ht="25.8" customHeight="1">
-      <c r="A6" t="s" s="10">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" ht="25.8" customHeight="1">
-      <c r="A7" t="s" s="10">
+      <c r="E15" s="11"/>
+      <c r="F15" s="11">
+        <v>22</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" ht="43.8" customHeight="1">
+      <c r="A16" s="12">
+        <f>A15+1</f>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s" s="14">
+        <v>24</v>
+      </c>
+      <c r="C16" s="10">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11">
+        <v>2</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" ht="25.8" customHeight="1">
+      <c r="A17" s="12">
+        <f>A16+1</f>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C17" s="10">
+        <v>2</v>
+      </c>
+      <c r="D17" s="11">
+        <v>2</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" ht="25.8" customHeight="1">
+      <c r="A18" s="12">
+        <f>A17+1</f>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s" s="14">
+        <v>26</v>
+      </c>
+      <c r="C18" s="10">
+        <v>2</v>
+      </c>
+      <c r="D18" s="11">
+        <v>2</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" ht="43.8" customHeight="1">
+      <c r="A19" s="12">
+        <f>A18+1</f>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s" s="14">
+        <v>27</v>
+      </c>
+      <c r="C19" s="10">
+        <v>2</v>
+      </c>
+      <c r="D19" s="11">
+        <v>2</v>
+      </c>
+      <c r="E19" s="11">
+        <v>17</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+    </row>
+    <row r="20" ht="25.8" customHeight="1">
+      <c r="A20" s="12">
+        <f>A19+1</f>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s" s="14">
+        <v>28</v>
+      </c>
+      <c r="C20" s="10">
+        <v>3</v>
+      </c>
+      <c r="D20" s="11">
+        <v>2</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" ht="25.8" customHeight="1">
+      <c r="A21" s="12">
+        <f>A20+1</f>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s" s="14">
+        <v>29</v>
+      </c>
+      <c r="C21" s="10">
+        <v>3</v>
+      </c>
+      <c r="D21" s="11">
+        <v>2</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" ht="43.8" customHeight="1">
+      <c r="A22" s="12">
+        <f>A21+1</f>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s" s="14">
+        <v>30</v>
+      </c>
+      <c r="C22" s="10">
+        <v>3</v>
+      </c>
+      <c r="D22" s="11">
+        <v>2</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+    </row>
+    <row r="23" ht="25.8" customHeight="1">
+      <c r="A23" s="12">
+        <f>A22+1</f>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s" s="14">
+        <v>31</v>
+      </c>
+      <c r="C23" s="10">
+        <v>3</v>
+      </c>
+      <c r="D23" s="11">
+        <v>2</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" ht="25.8" customHeight="1">
+      <c r="A24" s="12">
+        <f>A23+1</f>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s" s="14">
+        <v>32</v>
+      </c>
+      <c r="C24" s="10">
+        <v>3</v>
+      </c>
+      <c r="D24" s="11">
+        <v>2</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+    </row>
+    <row r="25" ht="25.8" customHeight="1">
+      <c r="A25" s="12">
+        <f>A24+1</f>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s" s="14">
+        <v>33</v>
+      </c>
+      <c r="C25" s="10">
+        <v>3</v>
+      </c>
+      <c r="D25" s="11">
+        <v>2</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+    </row>
+    <row r="26" ht="25.8" customHeight="1">
+      <c r="A26" s="12">
+        <f>A25+1</f>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s" s="14">
+        <v>34</v>
+      </c>
+      <c r="C26" s="10">
+        <v>3</v>
+      </c>
+      <c r="D26" s="11">
+        <v>3</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" ht="25.8" customHeight="1">
+      <c r="A27" s="12">
+        <f>A26+1</f>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s" s="14">
+        <v>35</v>
+      </c>
+      <c r="C27" s="10">
+        <v>3</v>
+      </c>
+      <c r="D27" s="11">
+        <v>3</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" ht="25.8" customHeight="1">
+      <c r="A28" s="12">
+        <f>A27+1</f>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s" s="14">
+        <v>36</v>
+      </c>
+      <c r="C28" s="10">
+        <v>3</v>
+      </c>
+      <c r="D28" s="11">
+        <v>3</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+    </row>
+    <row r="29" ht="25.8" customHeight="1">
+      <c r="A29" s="12">
+        <f>A28+1</f>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s" s="14">
+        <v>37</v>
+      </c>
+      <c r="C29" s="10">
+        <v>3</v>
+      </c>
+      <c r="D29" s="11">
+        <v>3</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+    </row>
+    <row r="30" ht="25.8" customHeight="1">
+      <c r="A30" s="12">
+        <f>A29+1</f>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s" s="14">
+        <v>38</v>
+      </c>
+      <c r="C30" s="10">
+        <v>3</v>
+      </c>
+      <c r="D30" s="11">
+        <v>3</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+    </row>
+    <row r="31" ht="25.8" customHeight="1">
+      <c r="A31" s="12">
+        <f>A30+1</f>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s" s="14">
+        <v>39</v>
+      </c>
+      <c r="C31" s="10">
+        <v>3</v>
+      </c>
+      <c r="D31" s="11">
+        <v>3</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+    </row>
+    <row r="32" ht="25.8" customHeight="1">
+      <c r="A32" s="12">
+        <f>A31+1</f>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s" s="14">
+        <v>40</v>
+      </c>
+      <c r="C32" s="10">
+        <v>3</v>
+      </c>
+      <c r="D32" s="11">
+        <v>3</v>
+      </c>
+      <c r="E32" s="11">
+        <v>20</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+    </row>
+    <row r="33" ht="25.8" customHeight="1">
+      <c r="A33" s="12">
+        <f>A32+1</f>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s" s="14">
+        <v>41</v>
+      </c>
+      <c r="C33" s="10">
+        <v>4</v>
+      </c>
+      <c r="D33" s="11">
+        <v>3</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+    </row>
+    <row r="34" ht="25.8" customHeight="1">
+      <c r="A34" s="12">
+        <f>A33+1</f>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s" s="14">
+        <v>42</v>
+      </c>
+      <c r="C34" s="10">
+        <v>4</v>
+      </c>
+      <c r="D34" s="11">
+        <v>3</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" ht="25.8" customHeight="1">
+      <c r="A35" s="12">
+        <f>A34+1</f>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s" s="14">
+        <v>43</v>
+      </c>
+      <c r="C35" s="10">
+        <v>4</v>
+      </c>
+      <c r="D35" s="11">
+        <v>3</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+    </row>
+    <row r="36" ht="25.8" customHeight="1">
+      <c r="A36" s="12">
+        <f>A35+1</f>
+        <v>35</v>
+      </c>
+      <c r="B36" t="s" s="14">
+        <v>44</v>
+      </c>
+      <c r="C36" s="10">
+        <v>4</v>
+      </c>
+      <c r="D36" s="11">
+        <v>3</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+    </row>
+    <row r="37" ht="43.8" customHeight="1">
+      <c r="A37" s="12">
+        <f>A36+1</f>
+        <v>36</v>
+      </c>
+      <c r="B37" t="s" s="14">
+        <v>45</v>
+      </c>
+      <c r="C37" s="10">
+        <v>4</v>
+      </c>
+      <c r="D37" s="11">
+        <v>4</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+    </row>
+    <row r="38" ht="25.8" customHeight="1">
+      <c r="A38" s="12">
+        <f>A37+1</f>
+        <v>37</v>
+      </c>
+      <c r="B38" t="s" s="14">
+        <v>46</v>
+      </c>
+      <c r="C38" s="10">
+        <v>4</v>
+      </c>
+      <c r="D38" s="11">
+        <v>4</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+    </row>
+    <row r="39" ht="25.8" customHeight="1">
+      <c r="A39" s="12">
+        <f>A38+1</f>
+        <v>38</v>
+      </c>
+      <c r="B39" t="s" s="14">
+        <v>47</v>
+      </c>
+      <c r="C39" s="10">
+        <v>4</v>
+      </c>
+      <c r="D39" s="11">
+        <v>4</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+    </row>
+    <row r="40" ht="25.8" customHeight="1">
+      <c r="A40" s="12">
+        <f>A39+1</f>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s" s="14">
+        <v>48</v>
+      </c>
+      <c r="C40" s="10">
+        <v>4</v>
+      </c>
+      <c r="D40" s="11">
+        <v>4</v>
+      </c>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+    </row>
+    <row r="41" ht="25.8" customHeight="1">
+      <c r="A41" s="12">
+        <f>A40+1</f>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s" s="14">
+        <v>49</v>
+      </c>
+      <c r="C41" s="10">
+        <v>4</v>
+      </c>
+      <c r="D41" s="11">
+        <v>4</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+    </row>
+    <row r="42" ht="25.8" customHeight="1">
+      <c r="A42" s="12">
+        <f>A41+1</f>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s" s="14">
+        <v>50</v>
+      </c>
+      <c r="C42" s="10">
+        <v>4</v>
+      </c>
+      <c r="D42" s="11">
+        <v>4</v>
+      </c>
+      <c r="E42" s="11">
         <v>13</v>
       </c>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" ht="25.8" customHeight="1">
-      <c r="A8" t="s" s="10">
-        <v>14</v>
-      </c>
-      <c r="B8" s="8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" ht="25.8" customHeight="1">
-      <c r="A9" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="B9" s="8">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9">
-        <v>9</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" ht="25.8" customHeight="1">
-      <c r="A10" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="B10" s="8">
-        <v>2</v>
-      </c>
-      <c r="C10" s="9">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" ht="25.8" customHeight="1">
-      <c r="A11" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="B11" s="8">
-        <v>2</v>
-      </c>
-      <c r="C11" s="9">
-        <v>1</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" ht="25.8" customHeight="1">
-      <c r="A12" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="B12" s="8">
-        <v>2</v>
-      </c>
-      <c r="C12" s="9">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" ht="25.8" customHeight="1">
-      <c r="A13" t="s" s="10">
-        <v>19</v>
-      </c>
-      <c r="B13" s="8">
-        <v>2</v>
-      </c>
-      <c r="C13" s="9">
-        <v>1</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" ht="25.8" customHeight="1">
-      <c r="A14" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="B14" s="8">
-        <v>2</v>
-      </c>
-      <c r="C14" s="9">
-        <v>1</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" ht="25.8" customHeight="1">
-      <c r="A15" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="B15" s="8">
-        <v>2</v>
-      </c>
-      <c r="C15" s="9">
-        <v>1</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9">
-        <v>22</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" ht="43.8" customHeight="1">
-      <c r="A16" t="s" s="10">
-        <v>22</v>
-      </c>
-      <c r="B16" s="8">
-        <v>2</v>
-      </c>
-      <c r="C16" s="9">
-        <v>2</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" ht="25.8" customHeight="1">
-      <c r="A17" t="s" s="10">
-        <v>23</v>
-      </c>
-      <c r="B17" s="8">
-        <v>2</v>
-      </c>
-      <c r="C17" s="9">
-        <v>2</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" ht="25.8" customHeight="1">
-      <c r="A18" t="s" s="10">
-        <v>24</v>
-      </c>
-      <c r="B18" s="8">
-        <v>2</v>
-      </c>
-      <c r="C18" s="9">
-        <v>2</v>
-      </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" ht="43.8" customHeight="1">
-      <c r="A19" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="B19" s="8">
-        <v>2</v>
-      </c>
-      <c r="C19" s="9">
-        <v>2</v>
-      </c>
-      <c r="D19" s="9">
-        <v>17</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" ht="25.8" customHeight="1">
-      <c r="A20" t="s" s="10">
-        <v>26</v>
-      </c>
-      <c r="B20" s="8">
-        <v>3</v>
-      </c>
-      <c r="C20" s="9">
-        <v>2</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" ht="25.8" customHeight="1">
-      <c r="A21" t="s" s="10">
-        <v>27</v>
-      </c>
-      <c r="B21" s="8">
-        <v>3</v>
-      </c>
-      <c r="C21" s="9">
-        <v>2</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" ht="43.8" customHeight="1">
-      <c r="A22" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="B22" s="8">
-        <v>3</v>
-      </c>
-      <c r="C22" s="9">
-        <v>2</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" ht="25.8" customHeight="1">
-      <c r="A23" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="B23" s="8">
-        <v>3</v>
-      </c>
-      <c r="C23" s="9">
-        <v>2</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" ht="25.8" customHeight="1">
-      <c r="A24" t="s" s="10">
-        <v>30</v>
-      </c>
-      <c r="B24" s="8">
-        <v>3</v>
-      </c>
-      <c r="C24" s="9">
-        <v>2</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" ht="25.8" customHeight="1">
-      <c r="A25" t="s" s="10">
-        <v>31</v>
-      </c>
-      <c r="B25" s="8">
-        <v>3</v>
-      </c>
-      <c r="C25" s="9">
-        <v>2</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" ht="25.8" customHeight="1">
-      <c r="A26" t="s" s="10">
-        <v>32</v>
-      </c>
-      <c r="B26" s="8">
-        <v>3</v>
-      </c>
-      <c r="C26" s="9">
-        <v>3</v>
-      </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" ht="25.8" customHeight="1">
-      <c r="A27" t="s" s="10">
-        <v>33</v>
-      </c>
-      <c r="B27" s="8">
-        <v>3</v>
-      </c>
-      <c r="C27" s="9">
-        <v>3</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" ht="25.8" customHeight="1">
-      <c r="A28" t="s" s="10">
-        <v>34</v>
-      </c>
-      <c r="B28" s="8">
-        <v>3</v>
-      </c>
-      <c r="C28" s="9">
-        <v>3</v>
-      </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" ht="25.8" customHeight="1">
-      <c r="A29" t="s" s="10">
-        <v>35</v>
-      </c>
-      <c r="B29" s="8">
-        <v>3</v>
-      </c>
-      <c r="C29" s="9">
-        <v>3</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" ht="25.8" customHeight="1">
-      <c r="A30" t="s" s="10">
-        <v>36</v>
-      </c>
-      <c r="B30" s="8">
-        <v>3</v>
-      </c>
-      <c r="C30" s="9">
-        <v>3</v>
-      </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" ht="25.8" customHeight="1">
-      <c r="A31" t="s" s="10">
-        <v>37</v>
-      </c>
-      <c r="B31" s="8">
-        <v>3</v>
-      </c>
-      <c r="C31" s="9">
-        <v>3</v>
-      </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" ht="25.8" customHeight="1">
-      <c r="A32" t="s" s="10">
-        <v>38</v>
-      </c>
-      <c r="B32" s="8">
-        <v>3</v>
-      </c>
-      <c r="C32" s="9">
-        <v>3</v>
-      </c>
-      <c r="D32" s="9">
-        <v>20</v>
-      </c>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" ht="25.8" customHeight="1">
-      <c r="A33" t="s" s="10">
-        <v>39</v>
-      </c>
-      <c r="B33" s="8">
-        <v>4</v>
-      </c>
-      <c r="C33" s="9">
-        <v>3</v>
-      </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" ht="25.8" customHeight="1">
-      <c r="A34" t="s" s="10">
-        <v>40</v>
-      </c>
-      <c r="B34" s="8">
-        <v>4</v>
-      </c>
-      <c r="C34" s="9">
-        <v>3</v>
-      </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" ht="25.8" customHeight="1">
-      <c r="A35" t="s" s="10">
-        <v>41</v>
-      </c>
-      <c r="B35" s="8">
-        <v>4</v>
-      </c>
-      <c r="C35" s="9">
-        <v>3</v>
-      </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" ht="25.8" customHeight="1">
-      <c r="A36" t="s" s="10">
-        <v>42</v>
-      </c>
-      <c r="B36" s="8">
-        <v>4</v>
-      </c>
-      <c r="C36" s="9">
-        <v>3</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-    </row>
-    <row r="37" ht="43.8" customHeight="1">
-      <c r="A37" t="s" s="10">
-        <v>43</v>
-      </c>
-      <c r="B37" s="8">
-        <v>4</v>
-      </c>
-      <c r="C37" s="9">
-        <v>4</v>
-      </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-    </row>
-    <row r="38" ht="25.8" customHeight="1">
-      <c r="A38" t="s" s="10">
-        <v>44</v>
-      </c>
-      <c r="B38" s="8">
-        <v>4</v>
-      </c>
-      <c r="C38" s="9">
-        <v>4</v>
-      </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" ht="25.8" customHeight="1">
-      <c r="A39" t="s" s="10">
-        <v>45</v>
-      </c>
-      <c r="B39" s="8">
-        <v>4</v>
-      </c>
-      <c r="C39" s="9">
-        <v>4</v>
-      </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-    </row>
-    <row r="40" ht="25.8" customHeight="1">
-      <c r="A40" t="s" s="10">
-        <v>46</v>
-      </c>
-      <c r="B40" s="8">
-        <v>4</v>
-      </c>
-      <c r="C40" s="9">
-        <v>4</v>
-      </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-    </row>
-    <row r="41" ht="25.8" customHeight="1">
-      <c r="A41" t="s" s="10">
-        <v>47</v>
-      </c>
-      <c r="B41" s="8">
-        <v>4</v>
-      </c>
-      <c r="C41" s="9">
-        <v>4</v>
-      </c>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" ht="25.8" customHeight="1">
-      <c r="A42" t="s" s="10">
-        <v>48</v>
-      </c>
-      <c r="B42" s="8">
-        <v>4</v>
-      </c>
-      <c r="C42" s="9">
-        <v>4</v>
-      </c>
-      <c r="D42" s="9">
-        <v>13</v>
-      </c>
-      <c r="E42" s="9">
+      <c r="F42" s="11">
         <v>5</v>
       </c>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>